<commit_message>
Updated virospore_multiquant_magalie.Rmd to reflect new calculations for dilutions and added phage one-step growth curve to this repo
</commit_message>
<xml_diff>
--- a/Magalie_virospore_quant/Data/Annulus_Quant/20250311_annulus_multiquant_pilot.xlsx
+++ b/Magalie_virospore_quant/Data/Annulus_Quant/20250311_annulus_multiquant_pilot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joyobrien/GitHub/VirosporeQuant/Magalie_virospore_quant/Data/Annulus_Quant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB442EB0-DF7E-9041-A861-3FF34A3468EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08087311-192B-9348-8594-0C638F1D039B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58880" yWindow="3520" windowWidth="33880" windowHeight="23700" xr2:uid="{0A693B96-4B1C-5841-BA31-A20ACD553E7C}"/>
+    <workbookView xWindow="61840" yWindow="7920" windowWidth="33880" windowHeight="23700" xr2:uid="{0A693B96-4B1C-5841-BA31-A20ACD553E7C}"/>
   </bookViews>
   <sheets>
     <sheet name="mutliquant_pilot" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Sample</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t xml:space="preserve">Took some liberty with the distance from PFU becuae it was really hard to measure in this case </t>
+  </si>
+  <si>
+    <t>Distance_from_PFU_cm_correct</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02D69C-1C1B-8D45-BB09-A2013B557C5A}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,7 +467,7 @@
     <col min="7" max="7" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -486,8 +489,11 @@
       <c r="G1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -509,8 +515,11 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -532,8 +541,11 @@
       <c r="G3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -555,8 +567,11 @@
       <c r="G4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -578,8 +593,11 @@
       <c r="G5">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -601,8 +619,11 @@
       <c r="G6">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -624,8 +645,11 @@
       <c r="G7">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -647,8 +671,11 @@
       <c r="G8">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -670,8 +697,11 @@
       <c r="G9">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -692,6 +722,9 @@
       </c>
       <c r="G10">
         <v>0.8</v>
+      </c>
+      <c r="H10">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>